<commit_message>
nag lagay ako ng save option and topwindow pop up ng qr codee
</commit_message>
<xml_diff>
--- a/AccountDatabase.xlsx
+++ b/AccountDatabase.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1827,6 +1827,78 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>704525</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Facilitator</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>dada</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>pineda</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>kyla@gmail.com</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>237826</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>filipino</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Catholic</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Married</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>asdddd</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
biggest commit guys (sync this first)
</commit_message>
<xml_diff>
--- a/AccountDatabase.xlsx
+++ b/AccountDatabase.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1971,6 +1971,78 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>622229</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Facilitator</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>kyla</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>pineda</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>asdhads@gmail.com</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>09182388232</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>filipino</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Catholic</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Single</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>kyadl</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>sadasd</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
User Restriction Added and Update
</commit_message>
<xml_diff>
--- a/AccountDatabase.xlsx
+++ b/AccountDatabase.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2185,6 +2185,216 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>504837</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Facilitator</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>aaa</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>a@gmail.com</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>23423423423</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>asdasdasdasd</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Catholic</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Married</t>
+        </is>
+      </c>
+      <c r="K29" t="n">
+        <v>67</v>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>asasasdasds</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>158425</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Facilitator</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>sadasdasd</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>asdasdas</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>as@gmail.com</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>31432423423</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>dsfsdfdswfs</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>INC</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Single</t>
+        </is>
+      </c>
+      <c r="K30" t="n">
+        <v>34</v>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>sdfsdfsdfsdfsdf</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>329339</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Facilitator</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>aas</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>asdasda</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>sasd@gmail.com</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>12341134223</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>sdfsdfdsfsd</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>INC</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Married</t>
+        </is>
+      </c>
+      <c r="K31" t="n">
+        <v>213</v>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>asdasdasdasdasda</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
User restriction all goods
</commit_message>
<xml_diff>
--- a/AccountDatabase.xlsx
+++ b/AccountDatabase.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2605,6 +2605,76 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>990210</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Facilitator</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>a@gmail.com</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>78908908908</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>gujkhjkyhjghk</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Muslim</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Married</t>
+        </is>
+      </c>
+      <c r="K35" t="n">
+        <v>77</v>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>hhhhhhhhhhhh</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>hhhhhhhh</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
para sayo to jabilat
</commit_message>
<xml_diff>
--- a/AccountDatabase.xlsx
+++ b/AccountDatabase.xlsx
@@ -649,7 +649,7 @@
       </c>
       <c r="M3" s="2" t="inlineStr">
         <is>
-          <t>Kanal</t>
+          <t>Kantutan Street Lucena City</t>
         </is>
       </c>
       <c r="N3" s="2" t="inlineStr">
@@ -1520,7 +1520,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>34</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">

</xml_diff>